<commit_message>
More changes for raids
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/raid-monsters.xlsx
+++ b/resources/data-imports/Monsters/raid-monsters.xlsx
@@ -1028,13 +1028,13 @@
         <v>52</v>
       </c>
       <c r="AQ3">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="AR3">
         <v>0.15</v>
       </c>
       <c r="AS3">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="AT3">
         <v>1</v>
@@ -1299,7 +1299,7 @@
         <v>52</v>
       </c>
       <c r="AQ5">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="AR5">
         <v>0.05</v>
@@ -1436,7 +1436,7 @@
         <v>52</v>
       </c>
       <c r="AQ6">
-        <v>0.12</v>
+        <v>0.32</v>
       </c>
       <c r="AR6">
         <v>0.12</v>
@@ -1573,7 +1573,7 @@
         <v>52</v>
       </c>
       <c r="AQ7">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
       <c r="AR7">
         <v>0.16</v>
@@ -1710,13 +1710,13 @@
         <v>52</v>
       </c>
       <c r="AQ8">
-        <v>0.05</v>
+        <v>0.45</v>
       </c>
       <c r="AR8">
-        <v>0.04</v>
+        <v>0.14</v>
       </c>
       <c r="AS8">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="AT8">
         <v>1</v>

</xml_diff>

<commit_message>
Added a new feature type - giving an additional 10 sets
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/raid-monsters.xlsx
+++ b/resources/data-imports/Monsters/raid-monsters.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -164,10 +164,13 @@
     <t>life_stealing_resistance</t>
   </si>
   <si>
+    <t>only_for_location_type</t>
+  </si>
+  <si>
     <t>Shadow of The Creator</t>
   </si>
   <si>
-    <t>2208179050-4416358100</t>
+    <t>2208179027348-4416358054696</t>
   </si>
   <si>
     <t>Smugglers Coin</t>
@@ -179,7 +182,7 @@
     <t>Corrupted Pirate</t>
   </si>
   <si>
-    <t>2438027300-4876054600</t>
+    <t>2438027308409-4876054616818</t>
   </si>
   <si>
     <t>Lost Tome Of Spells</t>
@@ -188,7 +191,7 @@
     <t>Shade of The Creators Pain</t>
   </si>
   <si>
-    <t>2691800400-5383600800</t>
+    <t>2691800385265-5383600770530</t>
   </si>
   <si>
     <t>Shade Dust</t>
@@ -197,7 +200,7 @@
     <t>Shadow Cultist</t>
   </si>
   <si>
-    <t>3095113600-6190227200</t>
+    <t>3095113594180-6190227188360</t>
   </si>
   <si>
     <t>Scholars Necklace</t>
@@ -206,7 +209,7 @@
     <t>The Quartermaster</t>
   </si>
   <si>
-    <t>3452138750-6904277500</t>
+    <t>3452138744086-6904277488171</t>
   </si>
   <si>
     <t>The Quartermasters Severed Head</t>
@@ -215,7 +218,7 @@
     <t>Shadow Merchant</t>
   </si>
   <si>
-    <t>3850347200-7700694400</t>
+    <t>4000000000000-8000000000000</t>
   </si>
   <si>
     <t>Simple Gem Necklace</t>
@@ -224,16 +227,13 @@
     <t>Enraged Pirate Lacky</t>
   </si>
   <si>
-    <t>4000000000-8000000000</t>
-  </si>
-  <si>
     <t>Clean White Feather</t>
   </si>
   <si>
     <t>Shadow Thief</t>
   </si>
   <si>
-    <t>2000000000-4000000000</t>
+    <t>2000000000000-4000000000000</t>
   </si>
   <si>
     <t>Stolen Coin</t>
@@ -242,7 +242,7 @@
     <t>Living Ice sickle</t>
   </si>
   <si>
-    <t>6612658750-13225317500</t>
+    <t>6049434988096-12098869976191</t>
   </si>
   <si>
     <t>Husbands Wallet</t>
@@ -254,19 +254,19 @@
     <t>Frozen King Krampus</t>
   </si>
   <si>
-    <t>8000000000-16000000000</t>
+    <t>7000000000000-14000000000000</t>
   </si>
   <si>
     <t>Rabid Reindeer</t>
   </si>
   <si>
-    <t>7498167550-14996335100</t>
+    <t>6708547813507-13417095627014</t>
   </si>
   <si>
     <t>Haunting Snowman</t>
   </si>
   <si>
-    <t>5656854250-11313708500</t>
+    <t>5291502622130-10583005244259</t>
   </si>
   <si>
     <t>The Poets Walking Stick</t>
@@ -275,7 +275,7 @@
     <t>Lost Memory of Her Son</t>
   </si>
   <si>
-    <t>5039684200-10079368400</t>
+    <t>4820284528351-9640569056701</t>
   </si>
   <si>
     <t>Bottle of Frozen Tears</t>
@@ -284,7 +284,7 @@
     <t>Queens Knight of the Ice Rose</t>
   </si>
   <si>
-    <t>4489848200-8979696400</t>
+    <t>4391029277220-8782058554440</t>
   </si>
   <si>
     <t>Ice Stave of Hope</t>
@@ -296,43 +296,58 @@
     <t>Shadow Child of Time</t>
   </si>
   <si>
+    <t>8000000000000-16000000000000</t>
+  </si>
+  <si>
+    <t>Picture of the Wandering Cleric</t>
+  </si>
+  <si>
     <t>Delusional Memories</t>
   </si>
   <si>
     <t>Fated Dream of Tomorrow</t>
   </si>
   <si>
-    <t>8979696400-17959392800</t>
+    <t>8979696386475-17959392772950</t>
   </si>
   <si>
     <t>Judge of Emotion</t>
   </si>
   <si>
-    <t>10079368400-20158736800</t>
+    <t>10079368399159-20158736798318</t>
+  </si>
+  <si>
+    <t>Journal of another time</t>
   </si>
   <si>
     <t>Kalitore the Gold Dragon</t>
   </si>
   <si>
-    <t>11313708500-22627417000</t>
+    <t>11313708498985-22627416997970</t>
   </si>
   <si>
     <t>Faceless Barbarian of Rage</t>
   </si>
   <si>
-    <t>13225317500-26450635000</t>
+    <t>13225317516437-26450635032873</t>
+  </si>
+  <si>
+    <t>Old bloody rusty knife</t>
   </si>
   <si>
     <t>Blind Prophet of The Church</t>
   </si>
   <si>
-    <t>14996335150-29992670300</t>
+    <t>14996335142329-29992670284658</t>
   </si>
   <si>
     <t>Bloody Bishop of Corrupted Alchemy</t>
   </si>
   <si>
-    <t>16000000000-32000000000</t>
+    <t>16000000000000-32000000000000</t>
+  </si>
+  <si>
+    <t>Silver Blade of Time</t>
   </si>
 </sst>
 </file>
@@ -672,7 +687,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AW23"/>
+  <dimension ref="A1:AX23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -682,14 +697,14 @@
   <cols>
     <col min="1" max="1" width="4.57" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="41.133" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="13" max="13" width="8.141" bestFit="true" customWidth="true" style="0"/>
@@ -702,10 +717,10 @@
     <col min="20" max="20" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="21" max="21" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="22" max="22" width="12.854" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="24" max="24" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="35.277" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="35.277" bestFit="true" customWidth="true" style="0"/>
     <col min="27" max="27" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="28" max="28" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="29" max="29" width="22.28" bestFit="true" customWidth="true" style="0"/>
@@ -729,9 +744,10 @@
     <col min="47" max="47" width="15.282" bestFit="true" customWidth="true" style="0"/>
     <col min="48" max="48" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="49" max="49" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="50" max="50" width="26.993" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:50">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -879,37 +895,40 @@
       <c r="AW1" t="s">
         <v>48</v>
       </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:50">
       <c r="A2">
         <v>368</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="D2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="E2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="F2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="G2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="H2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="I2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="J2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="K2">
         <v>0.0027</v>
@@ -945,22 +964,22 @@
         <v>0.0027</v>
       </c>
       <c r="W2">
-        <v>2208179050</v>
+        <v>2208179027348</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Z2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AA2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="AB2">
-        <v>4416358100</v>
+        <v>4416358054696</v>
       </c>
       <c r="AC2">
         <v>0.0027</v>
@@ -993,13 +1012,13 @@
         <v>1</v>
       </c>
       <c r="AM2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AN2">
         <v>0.05</v>
       </c>
       <c r="AO2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ2">
         <v>0.1829</v>
@@ -1017,36 +1036,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:50">
       <c r="A3">
         <v>369</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="D3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="E3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="F3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="G3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="H3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="I3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="J3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="K3">
         <v>0.0072</v>
@@ -1082,22 +1101,22 @@
         <v>0.0072</v>
       </c>
       <c r="W3">
-        <v>2438027300</v>
+        <v>2438027308409</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Z3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AA3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="AB3">
-        <v>4876054600</v>
+        <v>4876054616818</v>
       </c>
       <c r="AC3">
         <v>0.0072</v>
@@ -1130,13 +1149,13 @@
         <v>1</v>
       </c>
       <c r="AM3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AN3">
         <v>0.01</v>
       </c>
       <c r="AO3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ3">
         <v>0.2229</v>
@@ -1154,36 +1173,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:50">
       <c r="A4">
         <v>370</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="D4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="E4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="F4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="G4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="H4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="I4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="J4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="K4">
         <v>0.0193</v>
@@ -1219,22 +1238,22 @@
         <v>0.0193</v>
       </c>
       <c r="W4">
-        <v>2691800400</v>
+        <v>2691800385265</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Z4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AA4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="AB4">
-        <v>5383600800</v>
+        <v>5383600770530</v>
       </c>
       <c r="AC4">
         <v>0.0193</v>
@@ -1267,13 +1286,13 @@
         <v>1</v>
       </c>
       <c r="AM4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AN4">
         <v>0.01</v>
       </c>
       <c r="AO4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ4">
         <v>0.2717</v>
@@ -1291,36 +1310,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:50">
       <c r="A5">
         <v>371</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="D5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="E5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="F5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="G5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="H5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="I5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="J5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="K5">
         <v>0.0539</v>
@@ -1356,22 +1375,22 @@
         <v>0.0539</v>
       </c>
       <c r="W5">
-        <v>3095113600</v>
+        <v>3095113594180</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="AB5">
-        <v>6190227200</v>
+        <v>6190227188360</v>
       </c>
       <c r="AC5">
         <v>0.0539</v>
@@ -1404,13 +1423,13 @@
         <v>1</v>
       </c>
       <c r="AM5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AN5">
         <v>0.01</v>
       </c>
       <c r="AO5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ5">
         <v>0.3449</v>
@@ -1428,36 +1447,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:50">
       <c r="A6">
         <v>372</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="D6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="E6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="F6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="G6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="H6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="I6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="J6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="K6">
         <v>0.1462</v>
@@ -1493,22 +1512,22 @@
         <v>0.1462</v>
       </c>
       <c r="W6">
-        <v>3452138750</v>
+        <v>3452138744086</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Z6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="AB6">
-        <v>6904277500</v>
+        <v>6904277488171</v>
       </c>
       <c r="AC6">
         <v>0.1462</v>
@@ -1541,13 +1560,13 @@
         <v>1</v>
       </c>
       <c r="AM6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AN6">
         <v>0.01</v>
       </c>
       <c r="AO6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ6">
         <v>0.4248</v>
@@ -1565,36 +1584,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:50">
       <c r="A7">
         <v>373</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="D7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="E7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="F7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="G7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="H7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="I7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="J7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="K7">
         <v>0.3962</v>
@@ -1630,22 +1649,22 @@
         <v>0.3962</v>
       </c>
       <c r="W7">
-        <v>3850347200</v>
+        <v>4000000000000</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AA7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="AB7">
-        <v>7700694400</v>
+        <v>8000000000000</v>
       </c>
       <c r="AC7">
         <v>0.3962</v>
@@ -1678,13 +1697,13 @@
         <v>1</v>
       </c>
       <c r="AM7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AN7">
         <v>0.01</v>
       </c>
       <c r="AO7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ7">
         <v>0.5231</v>
@@ -1702,36 +1721,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:50">
       <c r="A8">
         <v>425</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="D8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="E8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="F8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="G8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="H8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="I8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="J8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1767,22 +1786,22 @@
         <v>1</v>
       </c>
       <c r="W8">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Z8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="AB8">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="AC8">
         <v>1</v>
@@ -1821,7 +1840,7 @@
         <v>0.01</v>
       </c>
       <c r="AO8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ8">
         <v>0.6</v>
@@ -1839,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:50">
       <c r="A9">
         <v>367</v>
       </c>
@@ -1847,28 +1866,28 @@
         <v>71</v>
       </c>
       <c r="C9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="D9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="E9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="F9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="G9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="H9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="I9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="J9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="K9">
         <v>0.001</v>
@@ -1904,7 +1923,7 @@
         <v>0.001</v>
       </c>
       <c r="W9">
-        <v>2000000000</v>
+        <v>2000000000000</v>
       </c>
       <c r="X9">
         <v>0</v>
@@ -1916,10 +1935,10 @@
         <v>72</v>
       </c>
       <c r="AA9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="AB9">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="AC9">
         <v>0.001</v>
@@ -1958,7 +1977,7 @@
         <v>1</v>
       </c>
       <c r="AO9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AQ9">
         <v>0.15</v>
@@ -1976,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:50">
       <c r="A10">
         <v>422</v>
       </c>
@@ -1984,28 +2003,28 @@
         <v>74</v>
       </c>
       <c r="C10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="D10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="E10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="F10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="G10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="H10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="I10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="J10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="K10">
         <v>0.1041</v>
@@ -2041,7 +2060,7 @@
         <v>0.1041</v>
       </c>
       <c r="W10">
-        <v>6612658750</v>
+        <v>6049434988096</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -2053,10 +2072,10 @@
         <v>75</v>
       </c>
       <c r="AA10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="AB10">
-        <v>13225317500</v>
+        <v>12098869976191</v>
       </c>
       <c r="AC10">
         <v>0.1041</v>
@@ -2113,7 +2132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:50">
       <c r="A11">
         <v>424</v>
       </c>
@@ -2121,28 +2140,28 @@
         <v>78</v>
       </c>
       <c r="C11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="D11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="E11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="F11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="G11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="H11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="I11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="J11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -2178,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="W11">
-        <v>8000000000</v>
+        <v>7000000000000</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -2190,10 +2209,10 @@
         <v>79</v>
       </c>
       <c r="AA11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="AB11">
-        <v>16000000000</v>
+        <v>14000000000000</v>
       </c>
       <c r="AC11">
         <v>1</v>
@@ -2244,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:50">
       <c r="A12">
         <v>423</v>
       </c>
@@ -2252,28 +2271,28 @@
         <v>80</v>
       </c>
       <c r="C12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="D12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="E12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="F12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="G12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="H12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="I12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="J12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="K12">
         <v>0.3327</v>
@@ -2309,7 +2328,7 @@
         <v>0.3327</v>
       </c>
       <c r="W12">
-        <v>7498167550</v>
+        <v>6708547813507</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -2321,10 +2340,10 @@
         <v>81</v>
       </c>
       <c r="AA12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="AB12">
-        <v>14996335100</v>
+        <v>13417095627014</v>
       </c>
       <c r="AC12">
         <v>0.3327</v>
@@ -2375,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:49">
+    <row r="13" spans="1:50">
       <c r="A13">
         <v>421</v>
       </c>
@@ -2383,28 +2402,28 @@
         <v>82</v>
       </c>
       <c r="C13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="D13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="E13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="F13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="G13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="H13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="I13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="J13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="K13">
         <v>0.0316</v>
@@ -2440,7 +2459,7 @@
         <v>0.0316</v>
       </c>
       <c r="W13">
-        <v>5656854250</v>
+        <v>5291502622130</v>
       </c>
       <c r="X13">
         <v>0</v>
@@ -2452,10 +2471,10 @@
         <v>83</v>
       </c>
       <c r="AA13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="AB13">
-        <v>11313708500</v>
+        <v>10583005244259</v>
       </c>
       <c r="AC13">
         <v>0.0316</v>
@@ -2512,7 +2531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:49">
+    <row r="14" spans="1:50">
       <c r="A14">
         <v>420</v>
       </c>
@@ -2520,28 +2539,28 @@
         <v>85</v>
       </c>
       <c r="C14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="D14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="E14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="F14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="G14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="H14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="I14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="J14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="K14">
         <v>0.01</v>
@@ -2577,7 +2596,7 @@
         <v>0.01</v>
       </c>
       <c r="W14">
-        <v>5039684200</v>
+        <v>4820284528351</v>
       </c>
       <c r="X14">
         <v>0</v>
@@ -2589,10 +2608,10 @@
         <v>86</v>
       </c>
       <c r="AA14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="AB14">
-        <v>10079368400</v>
+        <v>9640569056701</v>
       </c>
       <c r="AC14">
         <v>0.01</v>
@@ -2649,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49">
+    <row r="15" spans="1:50">
       <c r="A15">
         <v>419</v>
       </c>
@@ -2657,28 +2676,28 @@
         <v>88</v>
       </c>
       <c r="C15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="D15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="E15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="F15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="G15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="H15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="I15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="J15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="K15">
         <v>0.0032</v>
@@ -2714,7 +2733,7 @@
         <v>0.0032</v>
       </c>
       <c r="W15">
-        <v>4489848200</v>
+        <v>4391029277220</v>
       </c>
       <c r="X15">
         <v>0</v>
@@ -2726,10 +2745,10 @@
         <v>89</v>
       </c>
       <c r="AA15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="AB15">
-        <v>8979696400</v>
+        <v>8782058554440</v>
       </c>
       <c r="AC15">
         <v>0.0032</v>
@@ -2786,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:49">
+    <row r="16" spans="1:50">
       <c r="A16">
         <v>418</v>
       </c>
@@ -2794,28 +2813,28 @@
         <v>91</v>
       </c>
       <c r="C16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="D16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="E16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="F16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="G16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="H16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="I16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="J16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="K16">
         <v>0.001</v>
@@ -2851,22 +2870,22 @@
         <v>0.001</v>
       </c>
       <c r="W16">
-        <v>4000000000</v>
+        <v>4000000000000</v>
       </c>
       <c r="X16">
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="Z16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="AB16">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="AC16">
         <v>0.001</v>
@@ -2917,36 +2936,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:49">
+    <row r="17" spans="1:50">
       <c r="A17">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="B17" t="s">
         <v>92</v>
       </c>
       <c r="C17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="D17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="E17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="F17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="G17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="H17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="I17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="J17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="K17">
         <v>0.001</v>
@@ -2982,22 +3001,22 @@
         <v>0.001</v>
       </c>
       <c r="W17">
-        <v>8000000000</v>
+        <v>8000000000000</v>
       </c>
       <c r="X17">
         <v>0</v>
       </c>
       <c r="Y17" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="Z17" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="AA17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="AB17">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="AC17">
         <v>0.001</v>
@@ -3029,8 +3048,14 @@
       <c r="AL17">
         <v>1</v>
       </c>
+      <c r="AM17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AN17">
+        <v>0.05</v>
+      </c>
       <c r="AO17" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ17">
         <v>0.175</v>
@@ -3048,36 +3073,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:49">
+    <row r="18" spans="1:50">
       <c r="A18">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="D18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="E18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="F18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="G18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="H18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="I18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="J18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="K18">
         <v>0.0032</v>
@@ -3113,22 +3138,22 @@
         <v>0.0032</v>
       </c>
       <c r="W18">
-        <v>8979696400</v>
+        <v>8979696386475</v>
       </c>
       <c r="X18">
         <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="Z18" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="AA18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="AB18">
-        <v>17959392800</v>
+        <v>17959392772950</v>
       </c>
       <c r="AC18">
         <v>0.0032</v>
@@ -3161,7 +3186,7 @@
         <v>1</v>
       </c>
       <c r="AO18" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ18">
         <v>0.1955</v>
@@ -3179,36 +3204,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:49">
+    <row r="19" spans="1:50">
       <c r="A19">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="D19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="E19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="F19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="G19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="H19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="I19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="J19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="K19">
         <v>0.01</v>
@@ -3244,22 +3269,22 @@
         <v>0.01</v>
       </c>
       <c r="W19">
-        <v>10079368400</v>
+        <v>10079368399159</v>
       </c>
       <c r="X19">
         <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Z19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="AA19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="AB19">
-        <v>20158736800</v>
+        <v>20158736798318</v>
       </c>
       <c r="AC19">
         <v>0.01</v>
@@ -3291,8 +3316,14 @@
       <c r="AL19">
         <v>1</v>
       </c>
+      <c r="AM19" t="s">
+        <v>100</v>
+      </c>
+      <c r="AN19">
+        <v>0.07</v>
+      </c>
       <c r="AO19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ19">
         <v>0.2184</v>
@@ -3310,36 +3341,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:49">
+    <row r="20" spans="1:50">
       <c r="A20">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="D20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="E20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="F20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="G20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="H20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="I20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="J20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="K20">
         <v>0.0316</v>
@@ -3375,22 +3406,22 @@
         <v>0.0316</v>
       </c>
       <c r="W20">
-        <v>11313708500</v>
+        <v>11313708498985</v>
       </c>
       <c r="X20">
         <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="Z20" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="AA20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="AB20">
-        <v>22627417000</v>
+        <v>22627416997970</v>
       </c>
       <c r="AC20">
         <v>0.0316</v>
@@ -3423,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="AO20" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ20">
         <v>0.2439</v>
@@ -3441,36 +3472,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:49">
+    <row r="21" spans="1:50">
       <c r="A21">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="B21" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="D21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="E21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="F21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="G21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="H21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="I21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="J21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="K21">
         <v>0.1041</v>
@@ -3506,22 +3537,22 @@
         <v>0.1041</v>
       </c>
       <c r="W21">
-        <v>13225317500</v>
+        <v>13225317516437</v>
       </c>
       <c r="X21">
         <v>0</v>
       </c>
       <c r="Y21" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Z21" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="AA21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="AB21">
-        <v>26450635000</v>
+        <v>26450635032873</v>
       </c>
       <c r="AC21">
         <v>0.1041</v>
@@ -3553,8 +3584,14 @@
       <c r="AL21">
         <v>1</v>
       </c>
+      <c r="AM21" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN21">
+        <v>0.04</v>
+      </c>
       <c r="AO21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ21">
         <v>0.2838</v>
@@ -3572,36 +3609,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:49">
+    <row r="22" spans="1:50">
       <c r="A22">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="D22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="E22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="F22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="G22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="H22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="I22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="J22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="K22">
         <v>0.3327</v>
@@ -3637,22 +3674,22 @@
         <v>0.3327</v>
       </c>
       <c r="W22">
-        <v>14996335150</v>
+        <v>14996335142329</v>
       </c>
       <c r="X22">
         <v>0</v>
       </c>
       <c r="Y22" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Z22" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AA22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="AB22">
-        <v>29992670300</v>
+        <v>29992670284658</v>
       </c>
       <c r="AC22">
         <v>0.3327</v>
@@ -3685,7 +3722,7 @@
         <v>1</v>
       </c>
       <c r="AO22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ22">
         <v>0.3202</v>
@@ -3703,36 +3740,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:49">
+    <row r="23" spans="1:50">
       <c r="A23">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="D23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="E23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="F23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="G23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="H23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="I23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="J23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -3768,22 +3805,22 @@
         <v>1</v>
       </c>
       <c r="W23">
-        <v>16000000000</v>
+        <v>16000000000000</v>
       </c>
       <c r="X23">
         <v>0</v>
       </c>
       <c r="Y23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="Z23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="AA23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="AB23">
-        <v>32000000000</v>
+        <v>32000000000000</v>
       </c>
       <c r="AC23">
         <v>1</v>
@@ -3815,8 +3852,14 @@
       <c r="AL23">
         <v>1</v>
       </c>
+      <c r="AM23" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN23">
+        <v>0.09</v>
+      </c>
       <c r="AO23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="AQ23">
         <v>0.34</v>

</xml_diff>

<commit_message>
got new quest items for the raid and assigned some to the new raid monsters - in place
</commit_message>
<xml_diff>
--- a/resources/data-imports/Monsters/raid-monsters.xlsx
+++ b/resources/data-imports/Monsters/raid-monsters.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -248,6 +248,9 @@
     <t>25000000000-50000000000</t>
   </si>
   <si>
+    <t>Shield of Hope</t>
+  </si>
+  <si>
     <t>The Ice Plane</t>
   </si>
   <si>
@@ -257,12 +260,18 @@
     <t>24154721692-48309443384</t>
   </si>
   <si>
+    <t>Family Photo</t>
+  </si>
+  <si>
     <t>Faithless Prince of the Snow Garden</t>
   </si>
   <si>
     <t>21959370296-43918740591</t>
   </si>
   <si>
+    <t>Golden Pocket Watch</t>
+  </si>
+  <si>
     <t>Bloody Snowman of rage</t>
   </si>
   <si>
@@ -279,6 +288,9 @@
   </si>
   <si>
     <t>16333003332-32666006664</t>
+  </si>
+  <si>
+    <t>Locket of her hair</t>
   </si>
   <si>
     <t>Frozen Child of Fear</t>
@@ -2170,8 +2182,14 @@
       <c r="AL10">
         <v>0.8</v>
       </c>
+      <c r="AM10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN10">
+        <v>0.05</v>
+      </c>
       <c r="AO10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ10">
         <v>0.325</v>
@@ -2197,7 +2215,7 @@
         <v>560</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C11">
         <v>48309443384</v>
@@ -2263,10 +2281,10 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AA11">
         <v>48309443384</v>
@@ -2304,11 +2322,14 @@
       <c r="AL11">
         <v>0.3327</v>
       </c>
+      <c r="AM11" t="s">
+        <v>81</v>
+      </c>
       <c r="AN11">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="AO11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ11">
         <v>0.2916</v>
@@ -2334,7 +2355,7 @@
         <v>559</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C12">
         <v>43918740591</v>
@@ -2400,10 +2421,10 @@
         <v>0</v>
       </c>
       <c r="Y12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="Z12" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="AA12">
         <v>43918740591</v>
@@ -2441,11 +2462,14 @@
       <c r="AL12">
         <v>0.1041</v>
       </c>
+      <c r="AM12" t="s">
+        <v>84</v>
+      </c>
       <c r="AN12">
         <v>0.25</v>
       </c>
       <c r="AO12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ12">
         <v>0.2461</v>
@@ -2471,7 +2495,7 @@
         <v>558</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C13">
         <v>38729833463</v>
@@ -2537,10 +2561,10 @@
         <v>0</v>
       </c>
       <c r="Y13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Z13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="AA13">
         <v>38729833463</v>
@@ -2582,7 +2606,7 @@
         <v>0.58</v>
       </c>
       <c r="AO13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ13">
         <v>0.2016</v>
@@ -2608,7 +2632,7 @@
         <v>557</v>
       </c>
       <c r="B14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>35568933045</v>
@@ -2674,10 +2698,10 @@
         <v>0</v>
       </c>
       <c r="Y14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Z14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AA14">
         <v>35568933045</v>
@@ -2716,7 +2740,7 @@
         <v>0.01</v>
       </c>
       <c r="AO14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ14">
         <v>0.1719</v>
@@ -2742,7 +2766,7 @@
         <v>556</v>
       </c>
       <c r="B15" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C15">
         <v>32666006664</v>
@@ -2808,10 +2832,10 @@
         <v>0</v>
       </c>
       <c r="Y15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="Z15" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="AA15">
         <v>32666006664</v>
@@ -2849,8 +2873,14 @@
       <c r="AL15">
         <v>0.0032</v>
       </c>
+      <c r="AM15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN15">
+        <v>0.25</v>
+      </c>
       <c r="AO15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ15">
         <v>0.1466</v>
@@ -2876,7 +2906,7 @@
         <v>555</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C16">
         <v>30000000000</v>
@@ -2942,10 +2972,10 @@
         <v>0</v>
       </c>
       <c r="Y16" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="Z16" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="AA16">
         <v>30000000000</v>
@@ -2987,7 +3017,7 @@
         <v>0.1</v>
       </c>
       <c r="AO16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ16">
         <v>0.125</v>
@@ -3013,7 +3043,7 @@
         <v>424</v>
       </c>
       <c r="B17" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C17">
         <v>50000000000</v>
@@ -3121,7 +3151,7 @@
         <v>0.8</v>
       </c>
       <c r="AO17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ17">
         <v>0.325</v>
@@ -3147,7 +3177,7 @@
         <v>423</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C18">
         <v>46863547320</v>
@@ -3213,10 +3243,10 @@
         <v>0</v>
       </c>
       <c r="Y18" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="Z18" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="AA18">
         <v>46863547320</v>
@@ -3255,7 +3285,7 @@
         <v>0.3327</v>
       </c>
       <c r="AO18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ18">
         <v>0.2916</v>
@@ -3281,7 +3311,7 @@
         <v>422</v>
       </c>
       <c r="B19" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C19">
         <v>41329117239</v>
@@ -3347,10 +3377,10 @@
         <v>0</v>
       </c>
       <c r="Y19" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="Z19" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="AA19">
         <v>41329117239</v>
@@ -3389,13 +3419,13 @@
         <v>0.1041</v>
       </c>
       <c r="AM19" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="AN19">
         <v>0.1</v>
       </c>
       <c r="AO19" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ19">
         <v>0.2461</v>
@@ -3421,7 +3451,7 @@
         <v>421</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C20">
         <v>35355339060</v>
@@ -3487,10 +3517,10 @@
         <v>0</v>
       </c>
       <c r="Y20" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="Z20" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="AA20">
         <v>35355339060</v>
@@ -3529,13 +3559,13 @@
         <v>0.0316</v>
       </c>
       <c r="AM20" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="AN20">
         <v>0.58</v>
       </c>
       <c r="AO20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ20">
         <v>0.2016</v>
@@ -3561,7 +3591,7 @@
         <v>420</v>
       </c>
       <c r="B21" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C21">
         <v>31498026248</v>
@@ -3627,10 +3657,10 @@
         <v>0</v>
       </c>
       <c r="Y21" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="Z21" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="AA21">
         <v>31498026248</v>
@@ -3669,13 +3699,13 @@
         <v>0.01</v>
       </c>
       <c r="AM21" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="AN21">
         <v>0.25</v>
       </c>
       <c r="AO21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ21">
         <v>0.1719</v>
@@ -3701,7 +3731,7 @@
         <v>419</v>
       </c>
       <c r="B22" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C22">
         <v>28061551208</v>
@@ -3767,10 +3797,10 @@
         <v>0</v>
       </c>
       <c r="Y22" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Z22" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="AA22">
         <v>28061551208</v>
@@ -3809,13 +3839,13 @@
         <v>0.0032</v>
       </c>
       <c r="AM22" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="AN22">
         <v>0.1</v>
       </c>
       <c r="AO22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ22">
         <v>0.1466</v>
@@ -3841,7 +3871,7 @@
         <v>418</v>
       </c>
       <c r="B23" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C23">
         <v>25000000000</v>
@@ -3907,10 +3937,10 @@
         <v>0</v>
       </c>
       <c r="Y23" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="Z23" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="AA23">
         <v>25000000000</v>
@@ -3949,7 +3979,7 @@
         <v>0.001</v>
       </c>
       <c r="AO23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AQ23">
         <v>0.125</v>
@@ -3975,7 +4005,7 @@
         <v>518</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C24">
         <v>40000000000</v>
@@ -4041,10 +4071,10 @@
         <v>0</v>
       </c>
       <c r="Y24" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="Z24" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="AA24">
         <v>40000000000</v>
@@ -4083,13 +4113,13 @@
         <v>0.001</v>
       </c>
       <c r="AM24" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="AN24">
         <v>0.05</v>
       </c>
       <c r="AO24" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ24">
         <v>0.175</v>
@@ -4115,7 +4145,7 @@
         <v>519</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C25">
         <v>41787900317</v>
@@ -4181,10 +4211,10 @@
         <v>0</v>
       </c>
       <c r="Y25" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="Z25" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="AA25">
         <v>41787900317</v>
@@ -4223,7 +4253,7 @@
         <v>0.0032</v>
       </c>
       <c r="AO25" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ25">
         <v>0.1955</v>
@@ -4249,7 +4279,7 @@
         <v>520</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C26">
         <v>43655715323</v>
@@ -4315,10 +4345,10 @@
         <v>0</v>
       </c>
       <c r="Y26" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="Z26" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="AA26">
         <v>43655715323</v>
@@ -4357,13 +4387,13 @@
         <v>0.01</v>
       </c>
       <c r="AM26" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="AN26">
         <v>0.07</v>
       </c>
       <c r="AO26" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ26">
         <v>0.2184</v>
@@ -4389,7 +4419,7 @@
         <v>521</v>
       </c>
       <c r="B27" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C27">
         <v>45607017004</v>
@@ -4455,10 +4485,10 @@
         <v>0</v>
       </c>
       <c r="Y27" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="Z27" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="AA27">
         <v>45607017004</v>
@@ -4497,7 +4527,7 @@
         <v>0.0316</v>
       </c>
       <c r="AO27" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ27">
         <v>0.2439</v>
@@ -4523,7 +4553,7 @@
         <v>522</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C28">
         <v>49619419931</v>
@@ -4589,10 +4619,10 @@
         <v>0</v>
       </c>
       <c r="Y28" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="Z28" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="AA28">
         <v>49619419931</v>
@@ -4631,13 +4661,13 @@
         <v>0.1041</v>
       </c>
       <c r="AM28" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="AN28">
         <v>0.04</v>
       </c>
       <c r="AO28" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ28">
         <v>0.2838</v>
@@ -4663,7 +4693,7 @@
         <v>523</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C29">
         <v>52000000000</v>
@@ -4729,10 +4759,10 @@
         <v>0</v>
       </c>
       <c r="Y29" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="Z29" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="AA29">
         <v>50000000000</v>
@@ -4771,7 +4801,7 @@
         <v>0.3327</v>
       </c>
       <c r="AO29" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ29">
         <v>0.3202</v>
@@ -4797,7 +4827,7 @@
         <v>524</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C30">
         <v>52000000000</v>
@@ -4863,10 +4893,10 @@
         <v>0</v>
       </c>
       <c r="Y30" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="Z30" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="AA30">
         <v>50000000000</v>
@@ -4905,13 +4935,13 @@
         <v>0.8</v>
       </c>
       <c r="AM30" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="AN30">
         <v>0.09</v>
       </c>
       <c r="AO30" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="AQ30">
         <v>0.34</v>

</xml_diff>